<commit_message>
Changed code after code review + added httpx client
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,7 +617,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16.0.12026.20344</t>
+          <t>16.0.12130.20272</t>
         </is>
       </c>
     </row>
@@ -634,7 +634,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>16.0.12026.20344</t>
+          <t>16.0.12130.20272</t>
         </is>
       </c>
     </row>
@@ -692,92 +692,92 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Backup and Sync from Google</t>
+          <t>Microsoft Visual Studio Code Insiders</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Google, Inc.</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3.46.7395.1225</t>
+          <t>1.37.0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Microsoft Visual Studio Code Insiders</t>
+          <t>Logitech Gaming Software 5.10</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Logitech</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.37.0</t>
+          <t>5.10.127</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Logitech Gaming Software 5.10</t>
+          <t>Microsoft Visual C++ 2010  x64 Redistributable - 10.0.40219</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Logitech</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>5.10.127</t>
+          <t>10.0.40219</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2010  x64 Redistributable - 10.0.40219</t>
+          <t>Java 8 Update 201 (64-bit)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Oracle Corporation</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>10.0.40219</t>
+          <t>8.0.2010.9</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Java 8 Update 201 (64-bit)</t>
+          <t>Autodesk CAD Manager Tools</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Oracle Corporation</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>8.0.2010.9</t>
+          <t>16.0.0.65</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Autodesk CAD Manager Tools</t>
+          <t>Autodesk Civil View for 3ds Max 2020 64-bit</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -787,65 +787,65 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16.0.0.65</t>
+          <t>22.0.0.0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Autodesk Civil View for 3ds Max 2020 64-bit</t>
+          <t>Autodesk Network License Manager</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Autodesk, Inc.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>22.0.0.0</t>
+          <t>11.14.1.3</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Autodesk Network License Manager</t>
+          <t>Microsoft SQL Server 2014 Express LocalDB</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Autodesk, Inc.</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>11.14.1.3</t>
+          <t>12.1.4100.1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Microsoft SQL Server 2014 Express LocalDB</t>
+          <t>NVIDIA mental ray and IRay feature plugins for 3ds Max 2020</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>12.1.4100.1</t>
+          <t>22.0.0.0</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NVIDIA mental ray and IRay feature plugins for 3ds Max 2020</t>
+          <t>Autodesk BIM 360 Glue AutoCAD 2019 Add-in 64 bit</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -855,14 +855,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>22.0.0.0</t>
+          <t>4.70.9</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Autodesk BIM 360 Glue AutoCAD 2019 Add-in 64 bit</t>
+          <t>Autodesk Inventor Server Engine for 3ds Max 2020</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -872,31 +872,31 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>4.70.9</t>
+          <t>21.0</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Autodesk Inventor Server Engine for 3ds Max 2020</t>
+          <t>Microsoft Visual C++ 2005 Redistributable (x64)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>21.0</t>
+          <t>8.0.59192</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2005 Redistributable (x64)</t>
+          <t>Microsoft Visual Studio Installer</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -906,109 +906,109 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>8.0.59192</t>
+          <t>2.3.2217.1010</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Microsoft Visual Studio Installer</t>
+          <t>CMake</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Kitware</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2.0.3297.403</t>
+          <t>3.13.2</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CMake</t>
+          <t>PaperPort Image Printer 64-bit</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Kitware</t>
+          <t>Nuance Communications, Inc.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>3.13.2</t>
+          <t>14.00.0000</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PaperPort Image Printer 64-bit</t>
+          <t>AMD Ryzen Master SDK</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nuance Communications, Inc.</t>
+          <t>Advanced Micro Devices, Inc.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>14.00.0000</t>
+          <t>1.4.0.0659</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AMD Ryzen Master SDK</t>
+          <t>MAXtoA for 3ds Max 2020</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Advanced Micro Devices, Inc.</t>
+          <t>Solid Angle</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1.4.0.0659</t>
+          <t>2.4.43.0</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MAXtoA for 3ds Max 2020</t>
+          <t>Oracle VM VirtualBox 6.0.4</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Solid Angle</t>
+          <t>Oracle Corporation</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2.4.43.0</t>
+          <t>6.0.4</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Oracle VM VirtualBox 6.0.4</t>
+          <t>Backup and Sync from Google</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Oracle Corporation</t>
+          <t>Google, Inc.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>6.0.4</t>
+          <t>3.47.7654.0300</t>
         </is>
       </c>
     </row>
@@ -1304,182 +1304,182 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Battle.net</t>
+          <t>Visual Studio Community 2017</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Blizzard Entertainment</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
+          <t>Microsoft Corporation</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>15.9.28307.905</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Battlelog Web Plugins</t>
+          <t>Battle.net</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>EA Digital Illusions CE AB</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>2.3.0</t>
-        </is>
-      </c>
+          <t>Blizzard Entertainment</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>ESN Sonar</t>
+          <t>Battlelog Web Plugins</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ESN Social Software AB</t>
+          <t>EA Digital Illusions CE AB</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.70.4</t>
+          <t>2.3.0</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Google Chrome</t>
+          <t>ESN Sonar</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Google LLC</t>
+          <t>ESN Social Software AB</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>78.0.3904.70</t>
+          <t>0.70.4</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Origin</t>
+          <t>Google Chrome</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Electronic Arts, Inc.</t>
+          <t>Google LLC</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>10.5.47.29954</t>
+          <t>78.0.3904.97</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Overwatch</t>
+          <t>Origin</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Blizzard Entertainment</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr"/>
+          <t>Electronic Arts, Inc.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>10.5.47.29954</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Rockstar Games Social Club</t>
+          <t>Overwatch</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Rockstar Games</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>1.2.4.1</t>
-        </is>
-      </c>
+          <t>Blizzard Entertainment</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Rockstar Games Social Club</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Valve Corporation</t>
+          <t>Rockstar Games</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2.10.91.91</t>
+          <t>1.2.4.1</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>TeamViewer 14</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>TeamViewer</t>
+          <t>Valve Corporation</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>14.7.1965</t>
+          <t>2.10.91.91</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Tekken 7</t>
+          <t>TeamViewer 14</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>R.G. Mechanics, Panky</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr"/>
+          <t>TeamViewer</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>14.7.1965</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Uplay</t>
+          <t>Tekken 7</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ubisoft</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>29.0</t>
-        </is>
-      </c>
+          <t>R.G. Mechanics, Panky</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Assassin's Creed IV Black Flag</t>
+          <t>Uplay</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1487,12 +1487,16 @@
           <t>Ubisoft</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>29.0</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Assassin's Creed Unity RU</t>
+          <t>Assassin's Creed IV Black Flag</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1505,24 +1509,20 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2013 Redistributable (x64) - 12.0.30501</t>
+          <t>Assassin's Creed Unity RU</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>12.0.30501.0</t>
-        </is>
-      </c>
+          <t>Ubisoft</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Microsoft System CLR Types для SQL Server 2019 CTP2.2</t>
+          <t>Microsoft Visual C++ 2013 Redistributable (x64) - 12.0.30501</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1532,31 +1532,31 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>15.0.1200.24</t>
+          <t>12.0.30501.0</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Autodesk Material Library Base Resolution Image Library 2020</t>
+          <t>Microsoft System CLR Types для SQL Server 2019 CTP2.2</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>18.11.1.0</t>
+          <t>15.0.1200.24</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Autodesk ReCap Photo Update 19.1.0</t>
+          <t>Autodesk Material Library Base Resolution Image Library 2020</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1566,31 +1566,31 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>19.1.0.10</t>
+          <t>18.11.1.0</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MSXML 4.0 SP3 Parser</t>
+          <t>Autodesk ReCap Photo Update 19.1.0</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>4.30.2100.0</t>
+          <t>19.1.0.10</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Windows SDK AddOn</t>
+          <t>MSXML 4.0 SP3 Parser</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1600,133 +1600,133 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>10.1.0.0</t>
+          <t>4.30.2100.0</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Nuance PDF Viewer Plus</t>
+          <t>Windows SDK AddOn</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Nuance Communications, Inc</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>5.30.3290</t>
+          <t>10.1.0.0</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Nuance PaperPort 12</t>
+          <t>Nuance PDF Viewer Plus</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Nuance Communications, Inc.</t>
+          <t>Nuance Communications, Inc</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>12.1.0006</t>
+          <t>5.30.3290</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2017 Redistributable (x86) - 14.16.27024</t>
+          <t>Nuance PaperPort 12</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Nuance Communications, Inc.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>14.16.27024.1</t>
+          <t>12.1.0006</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Autodesk Genuine Service</t>
+          <t>Microsoft Visual C++ 2017 Redistributable (x86) - 14.16.27024</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>3.0.11</t>
+          <t>14.16.27024.1</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Battlefield™ 1</t>
+          <t>Autodesk Genuine Service</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Electronic Arts</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1.0.57.44284</t>
+          <t>3.0.11</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2012 Redistributable (x86) - 11.0.61030</t>
+          <t>Battlefield™ 1</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Electronic Arts</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>11.0.61030.0</t>
+          <t>1.0.57.44284</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Autodesk Material Library Base Resolution Image Library 2019</t>
+          <t>Microsoft Visual C++ 2012 Redistributable (x86) - 11.0.61030</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>17.11.3.0</t>
+          <t>11.0.61030.0</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Autodesk AutoCAD Performance Feedback Tool 1.3.0</t>
+          <t>Autodesk Material Library Base Resolution Image Library 2019</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1736,82 +1736,82 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1.3.0.0</t>
+          <t>17.11.3.0</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Chocolatey GUI</t>
+          <t>Autodesk AutoCAD Performance Feedback Tool 1.3.0</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Chocolatey</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>0.16.0.0</t>
+          <t>1.3.0.0</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Titanfall™ 2</t>
+          <t>Chocolatey GUI</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Electronic Arts, Inc.</t>
+          <t>Chocolatey</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>1.0.1.3</t>
+          <t>0.16.0.0</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>олосовой помощник Алиса</t>
+          <t>Titanfall™ 2</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Яндекс</t>
+          <t>Electronic Arts, Inc.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>5.0.0.1903</t>
+          <t>1.0.1.3</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2017 Redistributable (x64) - 14.16.27024</t>
+          <t>олосовой помощник Алиса</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Яндекс</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>14.16.27024.1</t>
+          <t>5.0.0.1903</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Windows Software Development Kit - Windows 10.0.17763.132</t>
+          <t>Microsoft Visual C++ 2017 Redistributable (x64) - 14.16.27024</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1821,14 +1821,14 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>10.1.17763.132</t>
+          <t>14.16.27024.1</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2005 Redistributable</t>
+          <t>Windows Software Development Kit - Windows 10.0.17763.132</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1838,150 +1838,150 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>8.0.61001</t>
+          <t>10.1.17763.132</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>екомендованные приложения Autodesk 2016-2019</t>
+          <t>Microsoft Visual C++ 2005 Redistributable</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2.5.0</t>
+          <t>8.0.61001</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>OEM Application Profile</t>
+          <t>екомендованные приложения Autodesk 2016-2019</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>азвание организации</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>1.00.0000</t>
+          <t>2.5.0</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Autodesk Download Manager</t>
+          <t>OEM Application Profile</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Autodesk, Inc.</t>
+          <t>азвание организации</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>6.1.32.0</t>
+          <t>1.00.0000</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>MSI Command Center</t>
+          <t>Autodesk Download Manager</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>MSI</t>
+          <t>Autodesk, Inc.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>3.0.0.87</t>
+          <t>6.1.32.0</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Realtek Ethernet Controller Driver</t>
+          <t>MSI Command Center</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Realtek</t>
+          <t>MSI</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>10.31.828.2018</t>
+          <t>3.0.0.87</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Autodesk Material Library 2019</t>
+          <t>Realtek Ethernet Controller Driver</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Realtek</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>17.11.3.0</t>
+          <t>10.31.828.2018</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>MSI MysticLight</t>
+          <t>Autodesk Material Library 2019</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>MSI</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>3.0.0.44</t>
+          <t>17.11.3.0</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2008 Redistributable - x86 9.0.30729.17</t>
+          <t>MSI MysticLight</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>MSI</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>9.0.30729</t>
+          <t>3.0.0.44</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2008 Redistributable - x86 9.0.30729.6161</t>
+          <t>Microsoft Visual C++ 2008 Redistributable - x86 9.0.30729.17</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -1991,116 +1991,116 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>9.0.30729.6161</t>
+          <t>9.0.30729</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Epic Games Launcher</t>
+          <t>Microsoft Visual C++ 2008 Redistributable - x86 9.0.30729.6161</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Epic Games, Inc.</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>1.1.167.0</t>
+          <t>9.0.30729.6161</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Battlefield 4™</t>
+          <t>Epic Games Launcher</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Electronic Arts</t>
+          <t>Epic Games, Inc.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>1.8.2.48475</t>
+          <t>1.1.167.0</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Dell Display Manager</t>
+          <t>Battlefield 4™</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>EnTech Taiwan</t>
+          <t>Electronic Arts</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>1.40</t>
+          <t>1.8.2.48475</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Autodesk Material Library Medium Resolution Image Library 2020</t>
+          <t>Dell Display Manager</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>EnTech Taiwan</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>18.11.1.0</t>
+          <t>1.40</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>UBitMenu RU</t>
+          <t>Autodesk Material Library Medium Resolution Image Library 2020</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>UBit Schweiz AG</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>01.04</t>
+          <t>18.11.1.0</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Autodesk Material Library 2020</t>
+          <t>UBitMenu RU</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>UBit Schweiz AG</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>18.11.1.0</t>
+          <t>01.04</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Autodesk App Manager 2016-2019</t>
+          <t>Autodesk Material Library 2020</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2110,31 +2110,31 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2.5.0</t>
+          <t>18.11.1.0</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2012 Redistributable (x64) - 11.0.61030</t>
+          <t>Autodesk App Manager 2016-2019</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>11.0.61030.0</t>
+          <t>2.5.0</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Microsoft XNA Framework Redistributable 4.0 Refresh</t>
+          <t>Microsoft Visual C++ 2012 Redistributable (x64) - 11.0.61030</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2144,14 +2144,14 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>4.0.30901.0</t>
+          <t>11.0.61030.0</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2010  x86 Redistributable - 10.0.40219</t>
+          <t>Microsoft XNA Framework Redistributable 4.0 Refresh</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2161,260 +2161,277 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>10.0.40219</t>
+          <t>4.0.30901.0</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Realtek High Definition Audio Driver</t>
+          <t>Microsoft Visual C++ 2010  x86 Redistributable - 10.0.40219</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Realtek Semiconductor Corp.</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>6.0.1.8581</t>
+          <t>10.0.40219</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Autodesk AutoCAD 2019.1.2 Update</t>
+          <t>Realtek High Definition Audio Driver</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Autodesk</t>
+          <t>Realtek Semiconductor Corp.</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>23.0.162.0</t>
+          <t>6.0.1.8581</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Microsoft Visual C++ 2013 Redistributable (x86) - 12.0.30501</t>
+          <t>Autodesk AutoCAD 2019.1.2 Update</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Microsoft Corporation</t>
+          <t>Autodesk</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>12.0.30501.0</t>
+          <t>23.0.162.0</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Brother MFL-Pro Suite DCP-L2520DW series</t>
+          <t>Microsoft Visual C++ 2013 Redistributable (x86) - 12.0.30501</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Brother Industries, Ltd.</t>
+          <t>Microsoft Corporation</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>1.0.2.0</t>
+          <t>12.0.30501.0</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Python Launcher</t>
+          <t>Brother MFL-Pro Suite DCP-L2520DW series</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Python Software Foundation</t>
+          <t>Brother Industries, Ltd.</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>3.7.6565.0</t>
+          <t>1.0.2.0</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>FARO LS 1.1.700.0 (64bit)</t>
+          <t>Python Launcher</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>FARO Scanner Production</t>
+          <t>Python Software Foundation</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>7.0.0.23</t>
+          <t>3.7.6565.0</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Discord</t>
+          <t>FARO LS 1.1.700.0 (64bit)</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Discord Inc.</t>
+          <t>FARO Scanner Production</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>0.0.305</t>
+          <t>7.0.0.23</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>GitKraken</t>
+          <t>Discord</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Axosoft, LLC</t>
+          <t>Discord Inc.</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>6.2.1</t>
+          <t>0.0.305</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Postman-win64-7.10.0</t>
+          <t>GitKraken</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Postman</t>
+          <t>Axosoft, LLC</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>7.10.0</t>
+          <t>6.2.1</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>JetBrains Toolbox</t>
+          <t>Postman-win64-7.11.0</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>JetBrains</t>
+          <t>Postman</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>1.12.4481</t>
+          <t>7.11.0</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>µTorrent</t>
+          <t>JetBrains Toolbox</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>BitTorrent Inc.</t>
+          <t>JetBrains</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>3.5.5.45146</t>
+          <t>1.12.4481</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Yandex</t>
+          <t>µTorrent</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t xml:space="preserve"> «ЯНДЕКС»</t>
+          <t>BitTorrent Inc.</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>19.10.0.1522</t>
+          <t>3.5.5.45146</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Python 3.7.2 (32-bit)</t>
+          <t>Yandex</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Python Software Foundation</t>
+          <t xml:space="preserve"> «ЯНДЕКС»</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>3.7.2150.0</t>
+          <t>19.10.2.195</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Qt</t>
+          <t>Python 3.7.2 (32-bit)</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>The Qt Company Ltd</t>
+          <t>Python Software Foundation</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>%MAINTENANCE_TOOL_VERSION%</t>
+          <t>3.7.2150.0</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
+          <t>Qt</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>The Qt Company Ltd</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>%MAINTENANCE_TOOL_VERSION%</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
           <t>Telegram Desktop version 1.8.15</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
+      <c r="B124" t="inlineStr">
         <is>
           <t>Telegram FZ-LLC</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr">
+      <c r="C124" t="inlineStr">
         <is>
           <t>1.8.15</t>
         </is>

</xml_diff>